<commit_message>
added Level 1 examples
</commit_message>
<xml_diff>
--- a/src/16 Scientific Libraries/07 Spreadsheets/data/colored.xlsx
+++ b/src/16 Scientific Libraries/07 Spreadsheets/data/colored.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="writing to cells" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="writing colors to cells" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1" refMode="A1" iterate="0" iterateCount="100" iterateDelta="0.001"/>
@@ -33072,7 +33072,7 @@
   <sheetData>
     <row r="1" ht="21" customHeight="1" s="1">
       <c r="A1" s="2455" t="n"/>
-      <c r="B1" s="5269" t="n"/>
+      <c r="B1" s="2456" t="n"/>
       <c r="C1" s="2457" t="n"/>
       <c r="D1" s="2458" t="n"/>
       <c r="E1" s="2459" t="n"/>
@@ -33162,9 +33162,9 @@
       <c r="CK1" s="2543" t="n"/>
     </row>
     <row r="2" ht="21" customHeight="1" s="1">
-      <c r="A2" s="5270" t="n"/>
+      <c r="A2" s="2456" t="n"/>
       <c r="B2" s="2458" t="n"/>
-      <c r="C2" s="5271" t="n"/>
+      <c r="C2" s="2460" t="n"/>
       <c r="D2" s="2462" t="n"/>
       <c r="E2" s="2464" t="n"/>
       <c r="F2" s="2466" t="n"/>

</xml_diff>